<commit_message>
Adding pom and test data
</commit_message>
<xml_diff>
--- a/home/TestData.xlsx
+++ b/home/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>UserName</t>
   </si>
@@ -61,24 +61,19 @@
   </si>
   <si>
     <t>Fashion Sale</t>
+  </si>
+  <si>
+    <t>kame9454</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,16 +96,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -412,17 +405,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -430,8 +427,8 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>123</v>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -439,6 +436,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -446,72 +444,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>